<commit_message>
updates for requireents and use cases
</commit_message>
<xml_diff>
--- a/CS320-Spring2022Calendar.xlsx
+++ b/CS320-Spring2022Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A9D687-DE51-4192-9270-D87938501C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C116E74A-723B-4D4A-8CE2-E24B21AAD700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="486" windowWidth="22026" windowHeight="11184" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3972" yWindow="414" windowWidth="16488" windowHeight="11784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp22" sheetId="1" r:id="rId1"/>
@@ -168,21 +168,6 @@
 (Scrum Guide)</t>
   </si>
   <si>
-    <t>Lecture 8: Requirements, Use Cases
-(UD: Chapter 9)
-Use Case Exercise
-(in class)</t>
-  </si>
-  <si>
-    <t>User Requirements Exercise
-(in class)</t>
-  </si>
-  <si>
-    <t>Team Session:
-Use Cases
-(in class)</t>
-  </si>
-  <si>
     <t>A04: Individual MS2
 50% Progresss</t>
   </si>
@@ -228,27 +213,6 @@
 Git and Egit
 Part II
 (in class)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Team Session:
-Textual Analysis
-(in class)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A05: Team Use Cases due
-7:00 am
-(Google Doc)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -351,25 +315,6 @@
   </si>
   <si>
     <t>Mar / Apr</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Team Session:
-Analysis Model (UML)
-(in class)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A06: Team Domain Analysis and Design assigned</t>
-    </r>
   </si>
   <si>
     <t>A06: Team Domain Analysis and Design due
@@ -566,8 +511,67 @@
 (Marmoset)</t>
   </si>
   <si>
+    <t>Lecture 8:
+Use Cases
+(UD: Chapter 9)
+Use Case Exercise
+(in class)</t>
+  </si>
+  <si>
+    <t>Team Session:
+Team Project Use Cases
+(in class)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Session:
+Team Project Analysis Model (UML)
+(in class)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A06: Team Domain Analysis and Design assigned</t>
+    </r>
+  </si>
+  <si>
+    <t>Lecture 8:
+Requirements
+(UD: Chapter 9)
+ Requirements Exercise
+(in class)</t>
+  </si>
+  <si>
     <t>CS320: SW Engineering - Spring 2022 Schedule
-(as of 2-6-2022, subject to change)</t>
+(as of 2-17-2022, subject to change)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Session:
+Textual Analysis
+(in class)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A05: Team Use Cases due
+7:00 am
+(Google Doc)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1658,35 +1662,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1694,6 +1674,60 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1705,36 +1739,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2079,8 +2083,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2098,17 +2102,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="128" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="130"/>
+      <c r="A1" s="145" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="147"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
@@ -2138,10 +2142,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="134">
+      <c r="A3" s="138">
         <v>15</v>
       </c>
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="129" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="113">
@@ -2173,8 +2177,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="133"/>
-      <c r="B4" s="150"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="132"/>
       <c r="C4" s="115" t="s">
         <v>8</v>
       </c>
@@ -2200,12 +2204,12 @@
       <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="133">
+      <c r="A5" s="139">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="138" t="s">
-        <v>56</v>
+      <c r="B5" s="130" t="s">
+        <v>52</v>
       </c>
       <c r="C5" s="8">
         <f>I3 + 1</f>
@@ -2236,30 +2240,30 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="135"/>
-      <c r="B6" s="139"/>
+      <c r="A6" s="142"/>
+      <c r="B6" s="131"/>
       <c r="C6" s="68"/>
       <c r="D6" s="62" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E6" s="86"/>
       <c r="F6" s="23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G6" s="67" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I6" s="69"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="136">
+      <c r="A7" s="143">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="140" t="s">
+      <c r="B7" s="150" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="51">
@@ -2292,30 +2296,30 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="137"/>
-      <c r="B8" s="141"/>
+      <c r="A8" s="136"/>
+      <c r="B8" s="151"/>
       <c r="C8" s="40" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="48" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="137">
+      <c r="A9" s="136">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="141"/>
+      <c r="B9" s="151"/>
       <c r="C9" s="15">
         <f>I7 + 1</f>
         <v>13</v>
@@ -2345,11 +2349,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="137"/>
-      <c r="B10" s="141"/>
+    <row r="10" spans="1:9" ht="90.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="136"/>
+      <c r="B10" s="151"/>
       <c r="C10" s="67" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="48" t="s">
         <v>25</v>
@@ -2360,16 +2364,16 @@
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="137">
+      <c r="A11" s="136">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="141"/>
+      <c r="B11" s="151"/>
       <c r="C11" s="18">
         <f>I9 + 1</f>
         <v>20</v>
@@ -2400,17 +2404,17 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="90.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="137"/>
-      <c r="B12" s="141"/>
+      <c r="A12" s="136"/>
+      <c r="B12" s="151"/>
       <c r="C12" s="40" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="E12" s="63"/>
       <c r="F12" s="63" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="G12" s="85"/>
       <c r="H12" s="127" t="s">
@@ -2419,12 +2423,12 @@
       <c r="I12" s="126"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="142">
+      <c r="A13" s="152">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="151" t="s">
-        <v>57</v>
+      <c r="B13" s="133" t="s">
+        <v>53</v>
       </c>
       <c r="C13" s="18">
         <f>I11 + 1</f>
@@ -2454,29 +2458,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="143"/>
-      <c r="B14" s="152"/>
+    <row r="14" spans="1:9" ht="107.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A14" s="153"/>
+      <c r="B14" s="134"/>
       <c r="C14" s="38"/>
       <c r="D14" s="103" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="82"/>
       <c r="F14" s="64" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="G14" s="78"/>
       <c r="H14" s="49" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="134">
+      <c r="A15" s="138">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="74">
@@ -2509,22 +2513,22 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="135"/>
-      <c r="B16" s="139"/>
+      <c r="A16" s="142"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="77" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="100" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="118" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H16" s="119" t="str">
         <f>G16</f>
@@ -2614,7 +2618,7 @@
       <c r="C23" s="41"/>
       <c r="D23" s="30"/>
       <c r="E23" s="99" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
@@ -2666,19 +2670,19 @@
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="128" t="str">
+      <c r="A28" s="145" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2022 Schedule
-(as of 2-6-2022, subject to change)</v>
-      </c>
-      <c r="B28" s="129"/>
-      <c r="C28" s="129"/>
-      <c r="D28" s="129"/>
-      <c r="E28" s="129"/>
-      <c r="F28" s="129"/>
-      <c r="G28" s="129"/>
-      <c r="H28" s="129"/>
-      <c r="I28" s="130"/>
+(as of 2-17-2022, subject to change)</v>
+      </c>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="146"/>
+      <c r="I28" s="147"/>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="str">
@@ -2716,11 +2720,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="131">
+      <c r="A30" s="148">
         <f>A15</f>
         <v>9</v>
       </c>
-      <c r="B30" s="149" t="s">
+      <c r="B30" s="129" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="87">
@@ -2753,8 +2757,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="132"/>
-      <c r="B31" s="138"/>
+      <c r="A31" s="149"/>
+      <c r="B31" s="130"/>
       <c r="C31" s="87" t="str">
         <f>C16</f>
         <v xml:space="preserve"> </v>
@@ -2788,11 +2792,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="132">
+      <c r="A32" s="149">
         <f xml:space="preserve"> A30 - 1</f>
         <v>8</v>
       </c>
-      <c r="B32" s="138"/>
+      <c r="B32" s="130"/>
       <c r="C32" s="112">
         <f>I15 + 1</f>
         <v>13</v>
@@ -2823,10 +2827,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="133"/>
-      <c r="B33" s="138"/>
+      <c r="A33" s="139"/>
+      <c r="B33" s="130"/>
       <c r="C33" s="40" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>15</v>
@@ -2842,11 +2846,11 @@
       <c r="I33" s="47"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="133">
+      <c r="A34" s="139">
         <f>A32 - 1</f>
         <v>7</v>
       </c>
-      <c r="B34" s="138"/>
+      <c r="B34" s="130"/>
       <c r="C34" s="21">
         <f>I32 + 1</f>
         <v>20</v>
@@ -2877,29 +2881,29 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="120.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="133"/>
-      <c r="B35" s="138"/>
+      <c r="A35" s="139"/>
+      <c r="B35" s="130"/>
       <c r="C35" s="66"/>
       <c r="D35" s="33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E35" s="80"/>
       <c r="F35" s="60" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G35" s="66"/>
       <c r="H35" s="101" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I35" s="94"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="133">
+      <c r="A36" s="139">
         <f>A34 - 1</f>
         <v>6</v>
       </c>
-      <c r="B36" s="153" t="s">
-        <v>58</v>
+      <c r="B36" s="135" t="s">
+        <v>54</v>
       </c>
       <c r="C36" s="8">
         <f>I34 + 1</f>
@@ -2930,30 +2934,30 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="135"/>
-      <c r="B37" s="139"/>
+      <c r="A37" s="142"/>
+      <c r="B37" s="131"/>
       <c r="C37" s="93"/>
       <c r="D37" s="25" t="s">
         <v>29</v>
       </c>
       <c r="E37" s="67" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>30</v>
       </c>
       <c r="G37" s="94"/>
       <c r="H37" s="105" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I37" s="37"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="136">
+      <c r="A38" s="143">
         <f>A36 -1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="148" t="s">
+      <c r="B38" s="128" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="91">
@@ -2986,30 +2990,30 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="137"/>
-      <c r="B39" s="148"/>
+      <c r="A39" s="136"/>
+      <c r="B39" s="128"/>
       <c r="C39" s="96"/>
       <c r="D39" s="33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G39" s="104"/>
       <c r="H39" s="102" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="147">
+      <c r="A40" s="144">
         <f>A38 -1</f>
         <v>4</v>
       </c>
-      <c r="B40" s="148"/>
+      <c r="B40" s="128"/>
       <c r="C40" s="95">
         <f>I38 + 1</f>
         <v>10</v>
@@ -3040,8 +3044,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="44.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="137"/>
-      <c r="B41" s="148"/>
+      <c r="A41" s="136"/>
+      <c r="B41" s="128"/>
       <c r="C41" s="38"/>
       <c r="D41" s="36" t="s">
         <v>7</v>
@@ -3059,11 +3063,11 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="137">
+      <c r="A42" s="136">
         <f>A40 -1</f>
         <v>3</v>
       </c>
-      <c r="B42" s="148"/>
+      <c r="B42" s="128"/>
       <c r="C42" s="110">
         <f>I40 + 1</f>
         <v>17</v>
@@ -3094,8 +3098,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="137"/>
-      <c r="B43" s="148"/>
+      <c r="A43" s="136"/>
+      <c r="B43" s="128"/>
       <c r="C43" s="115" t="s">
         <v>6</v>
       </c>
@@ -3113,11 +3117,11 @@
       <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="137">
+      <c r="A44" s="136">
         <f>A42 -1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="148"/>
+      <c r="B44" s="128"/>
       <c r="C44" s="38">
         <f>I42 + 1</f>
         <v>24</v>
@@ -3148,8 +3152,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="144"/>
-      <c r="B45" s="148"/>
+      <c r="A45" s="137"/>
+      <c r="B45" s="128"/>
       <c r="C45" s="88"/>
       <c r="D45" s="57"/>
       <c r="E45" s="55"/>
@@ -3163,11 +3167,11 @@
       <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="134">
+      <c r="A46" s="138">
         <f>A44 -1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="149" t="s">
+      <c r="B46" s="129" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="34">
@@ -3199,8 +3203,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="133"/>
-      <c r="B47" s="138"/>
+      <c r="A47" s="139"/>
+      <c r="B47" s="130"/>
       <c r="C47" s="35"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -3211,17 +3215,17 @@
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I47" s="39" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="145" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" s="138"/>
+      <c r="A48" s="140" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="130"/>
       <c r="C48" s="21">
         <f>I46 + 1</f>
         <v>8</v>
@@ -3252,17 +3256,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A49" s="146"/>
-      <c r="B49" s="139"/>
+      <c r="A49" s="141"/>
+      <c r="B49" s="131"/>
       <c r="C49" s="97" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E49" s="98"/>
       <c r="F49" s="25" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="124"/>
@@ -3271,21 +3275,6 @@
     <row r="50" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -3299,6 +3288,21 @@
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="98" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
schedule changes for Winter Break week team sessions
</commit_message>
<xml_diff>
--- a/CS320-Spring2022Calendar.xlsx
+++ b/CS320-Spring2022Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C116E74A-723B-4D4A-8CE2-E24B21AAD700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6A88EA-1080-4332-BABB-57C25EB8A6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3972" yWindow="414" windowWidth="16488" windowHeight="11784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="468" windowWidth="17202" windowHeight="11484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp22" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>Monday</t>
   </si>
@@ -86,12 +86,6 @@
   <si>
     <t>Lecture 11: OO Design, OCP, LSP
 Design Principles and Design Patterns</t>
-  </si>
-  <si>
-    <t>Lecture 16: Testing</t>
-  </si>
-  <si>
-    <t>Lecture 17: Code Quality</t>
   </si>
   <si>
     <t>Lecture 1:
@@ -375,50 +369,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Lecture  15: ORM, Designing a Persistence Layer
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Lab 5: JDBC due
-7:00 am
-(Marmoset)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 6: ORM
-(assigned)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Library Example Project
 Analysis and
 Review (part 1)
@@ -482,30 +432,6 @@
 (in class)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Work Ethic Lecture</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Lab 6: ORM due  7:00 am (Marmoset)</t>
-    </r>
-  </si>
-  <si>
     <t>A02: Individual Project Proposal due
 7:00 am
 (Marmoset)</t>
@@ -547,10 +473,6 @@
 (UD: Chapter 9)
  Requirements Exercise
 (in class)</t>
-  </si>
-  <si>
-    <t>CS320: SW Engineering - Spring 2022 Schedule
-(as of 2-17-2022, subject to change)</t>
   </si>
   <si>
     <r>
@@ -572,6 +494,50 @@
 7:00 am
 (Google Doc)</t>
     </r>
+  </si>
+  <si>
+    <t>Team Session:
+Design &amp; MS1
+(in-class)</t>
+  </si>
+  <si>
+    <t>Lab 6: ORM due  7:00 am (Marmoset)</t>
+  </si>
+  <si>
+    <t>Lecture 16: Testing
+Lecture 17: Quality Assurance</t>
+  </si>
+  <si>
+    <t>Lab 5: JDBC due
+7:00 am
+(Marmoset)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lecture  15: ORM, Designing a Persistence Layer
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Lab 6: ORM
+(assigned)</t>
+    </r>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2022 Schedule
+(as of 2-23-2022, subject to change)</t>
+  </si>
+  <si>
+    <t>Work Ethic
+Lecture</t>
   </si>
 </sst>
 </file>
@@ -1581,9 +1547,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1593,9 +1556,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1660,6 +1620,66 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1668,12 +1688,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1686,58 +1700,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2083,8 +2049,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2102,21 +2068,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="145" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="147"/>
+      <c r="A1" s="126" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="128"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -2142,24 +2108,24 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="138">
+      <c r="A3" s="132">
         <v>15</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="113">
+      <c r="C3" s="111">
         <v>23</v>
       </c>
-      <c r="D3" s="107">
+      <c r="D3" s="105">
         <f>C3 + 1</f>
         <v>24</v>
       </c>
-      <c r="E3" s="107">
+      <c r="E3" s="105">
         <f t="shared" ref="E3:I3" si="0">D3 + 1</f>
         <v>25</v>
       </c>
-      <c r="F3" s="114">
+      <c r="F3" s="112">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
@@ -2177,39 +2143,39 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="139"/>
-      <c r="B4" s="132"/>
-      <c r="C4" s="115" t="s">
+      <c r="A4" s="131"/>
+      <c r="B4" s="148"/>
+      <c r="C4" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="110" t="str">
+      <c r="D4" s="108" t="str">
         <f xml:space="preserve"> C4</f>
         <v>SEMESTER
 BREAK</v>
       </c>
-      <c r="E4" s="116" t="str">
+      <c r="E4" s="114" t="str">
         <f>D4</f>
         <v>SEMESTER
 BREAK</v>
       </c>
-      <c r="F4" s="117" t="str">
+      <c r="F4" s="115" t="str">
         <f>E4</f>
         <v>SEMESTER
 BREAK</v>
       </c>
       <c r="G4" s="50"/>
       <c r="H4" s="49" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="139">
+      <c r="A5" s="131">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="130" t="s">
-        <v>52</v>
+      <c r="B5" s="136" t="s">
+        <v>50</v>
       </c>
       <c r="C5" s="8">
         <f>I3 + 1</f>
@@ -2240,30 +2206,30 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="142"/>
-      <c r="B6" s="131"/>
+      <c r="A6" s="133"/>
+      <c r="B6" s="137"/>
       <c r="C6" s="68"/>
       <c r="D6" s="62" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="86"/>
       <c r="F6" s="23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G6" s="67" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I6" s="69"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="143">
+      <c r="A7" s="134">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="150" t="s">
+      <c r="B7" s="138" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="51">
@@ -2296,30 +2262,30 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="136"/>
-      <c r="B8" s="151"/>
+      <c r="A8" s="135"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="136">
+      <c r="A9" s="135">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="151"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="15">
         <f>I7 + 1</f>
         <v>13</v>
@@ -2350,30 +2316,30 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="90.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="136"/>
-      <c r="B10" s="151"/>
+      <c r="A10" s="135"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="67" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="136">
+      <c r="A11" s="135">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="151"/>
+      <c r="B11" s="139"/>
       <c r="C11" s="18">
         <f>I9 + 1</f>
         <v>20</v>
@@ -2404,31 +2370,31 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="90.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="136"/>
-      <c r="B12" s="151"/>
+      <c r="A12" s="135"/>
+      <c r="B12" s="139"/>
       <c r="C12" s="40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E12" s="63"/>
       <c r="F12" s="63" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G12" s="85"/>
-      <c r="H12" s="127" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="126"/>
+      <c r="H12" s="125" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="124"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="152">
+      <c r="A13" s="140">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="133" t="s">
-        <v>53</v>
+      <c r="B13" s="149" t="s">
+        <v>51</v>
       </c>
       <c r="C13" s="18">
         <f>I11 + 1</f>
@@ -2459,28 +2425,28 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="107.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="153"/>
-      <c r="B14" s="134"/>
+      <c r="A14" s="141"/>
+      <c r="B14" s="150"/>
       <c r="C14" s="38"/>
-      <c r="D14" s="103" t="s">
-        <v>32</v>
+      <c r="D14" s="102" t="s">
+        <v>30</v>
       </c>
       <c r="E14" s="82"/>
       <c r="F14" s="64" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G14" s="78"/>
       <c r="H14" s="49" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="138">
+      <c r="A15" s="132">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="136" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="74">
@@ -2499,43 +2465,43 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="G15" s="109">
+      <c r="G15" s="107">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="H15" s="110">
+      <c r="H15" s="108">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="I15" s="111">
+      <c r="I15" s="109">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="142"/>
-      <c r="B16" s="131"/>
+      <c r="A16" s="133"/>
+      <c r="B16" s="137"/>
       <c r="C16" s="77" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="E16" s="100" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="118" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="119" t="str">
+        <v>67</v>
+      </c>
+      <c r="G16" s="116" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="117" t="str">
         <f>G16</f>
         <v>WINTER
 BREAK</v>
       </c>
-      <c r="I16" s="120" t="str">
+      <c r="I16" s="118" t="str">
         <f>H16</f>
         <v>WINTER
 BREAK</v>
@@ -2557,7 +2523,7 @@
       <c r="B18" s="27"/>
       <c r="D18" s="30"/>
       <c r="E18" s="46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
@@ -2568,8 +2534,8 @@
       <c r="A19" s="42"/>
       <c r="B19" s="32"/>
       <c r="D19" s="26"/>
-      <c r="E19" s="121" t="s">
-        <v>21</v>
+      <c r="E19" s="119" t="s">
+        <v>19</v>
       </c>
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
@@ -2581,7 +2547,7 @@
       <c r="B20" s="27"/>
       <c r="D20" s="30"/>
       <c r="E20" s="43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
@@ -2593,7 +2559,7 @@
       <c r="B21" s="27"/>
       <c r="D21" s="30"/>
       <c r="E21" s="44" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F21" s="30"/>
       <c r="G21" s="30"/>
@@ -2605,7 +2571,7 @@
       <c r="B22" s="27"/>
       <c r="D22" s="30"/>
       <c r="E22" s="45" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
@@ -2618,7 +2584,7 @@
       <c r="C23" s="41"/>
       <c r="D23" s="30"/>
       <c r="E23" s="99" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
@@ -2670,19 +2636,19 @@
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="145" t="str">
+      <c r="A28" s="126" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2022 Schedule
-(as of 2-17-2022, subject to change)</v>
-      </c>
-      <c r="B28" s="146"/>
-      <c r="C28" s="146"/>
-      <c r="D28" s="146"/>
-      <c r="E28" s="146"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
-      <c r="H28" s="146"/>
-      <c r="I28" s="147"/>
+(as of 2-23-2022, subject to change)</v>
+      </c>
+      <c r="B28" s="127"/>
+      <c r="C28" s="127"/>
+      <c r="D28" s="127"/>
+      <c r="E28" s="127"/>
+      <c r="F28" s="127"/>
+      <c r="G28" s="127"/>
+      <c r="H28" s="127"/>
+      <c r="I28" s="128"/>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="str">
@@ -2720,11 +2686,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="148">
+      <c r="A30" s="129">
         <f>A15</f>
         <v>9</v>
       </c>
-      <c r="B30" s="129" t="s">
+      <c r="B30" s="147" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="87">
@@ -2743,29 +2709,31 @@
         <f>F15</f>
         <v>9</v>
       </c>
-      <c r="G30" s="106">
+      <c r="G30" s="104">
         <f>G15</f>
         <v>10</v>
       </c>
-      <c r="H30" s="107">
+      <c r="H30" s="105">
         <f>H15</f>
         <v>11</v>
       </c>
-      <c r="I30" s="108">
+      <c r="I30" s="106">
         <f>I15</f>
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="149"/>
-      <c r="B31" s="130"/>
+      <c r="A31" s="130"/>
+      <c r="B31" s="136"/>
       <c r="C31" s="87" t="str">
         <f>C16</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D31" s="81" t="str">
         <f t="shared" ref="D31:H31" si="5">D16</f>
-        <v>Lecture 16: Testing</v>
+        <v>Team Session:
+Design &amp; MS1
+(in-class)</v>
       </c>
       <c r="E31" s="80" t="str">
         <f t="shared" si="5"/>
@@ -2773,31 +2741,33 @@
       </c>
       <c r="F31" s="81" t="str">
         <f t="shared" si="5"/>
-        <v>Lecture 17: Code Quality</v>
-      </c>
-      <c r="G31" s="109" t="str">
+        <v>Team Session:
+Design &amp; MS1
+(in-class)</v>
+      </c>
+      <c r="G31" s="107" t="str">
         <f t="shared" si="5"/>
         <v>WINTER
 BREAK</v>
       </c>
-      <c r="H31" s="110" t="str">
+      <c r="H31" s="108" t="str">
         <f t="shared" si="5"/>
         <v>WINTER
 BREAK</v>
       </c>
-      <c r="I31" s="111" t="str">
+      <c r="I31" s="109" t="str">
         <f>I16</f>
         <v>WINTER
 BREAK</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="149">
+      <c r="A32" s="130">
         <f xml:space="preserve"> A30 - 1</f>
         <v>8</v>
       </c>
-      <c r="B32" s="130"/>
-      <c r="C32" s="112">
+      <c r="B32" s="136"/>
+      <c r="C32" s="110">
         <f>I15 + 1</f>
         <v>13</v>
       </c>
@@ -2827,10 +2797,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="139"/>
-      <c r="B33" s="130"/>
+      <c r="A33" s="131"/>
+      <c r="B33" s="136"/>
       <c r="C33" s="40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>15</v>
@@ -2841,16 +2811,16 @@
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I33" s="47"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="139">
+      <c r="A34" s="131">
         <f>A32 - 1</f>
         <v>7</v>
       </c>
-      <c r="B34" s="130"/>
+      <c r="B34" s="136"/>
       <c r="C34" s="21">
         <f>I32 + 1</f>
         <v>20</v>
@@ -2881,29 +2851,31 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="120.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="139"/>
-      <c r="B35" s="130"/>
+      <c r="A35" s="131"/>
+      <c r="B35" s="136"/>
       <c r="C35" s="66"/>
       <c r="D35" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E35" s="80"/>
       <c r="F35" s="60" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G35" s="66"/>
-      <c r="H35" s="101" t="s">
-        <v>59</v>
-      </c>
-      <c r="I35" s="94"/>
+      <c r="H35" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35" s="153" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="139">
+      <c r="A36" s="131">
         <f>A34 - 1</f>
         <v>6</v>
       </c>
-      <c r="B36" s="135" t="s">
-        <v>54</v>
+      <c r="B36" s="151" t="s">
+        <v>52</v>
       </c>
       <c r="C36" s="8">
         <f>I34 + 1</f>
@@ -2934,30 +2906,32 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="142"/>
-      <c r="B37" s="131"/>
+      <c r="A37" s="133"/>
+      <c r="B37" s="137"/>
       <c r="C37" s="93"/>
       <c r="D37" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E37" s="67" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G37" s="94"/>
-      <c r="H37" s="105" t="s">
-        <v>64</v>
-      </c>
-      <c r="I37" s="37"/>
+      <c r="H37" s="152" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" s="39" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="143">
+      <c r="A38" s="134">
         <f>A36 -1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="128" t="s">
+      <c r="B38" s="146" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="91">
@@ -2990,30 +2964,30 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="136"/>
-      <c r="B39" s="128"/>
+      <c r="A39" s="135"/>
+      <c r="B39" s="146"/>
       <c r="C39" s="96"/>
       <c r="D39" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="G39" s="104"/>
-      <c r="H39" s="102" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="G39" s="103"/>
+      <c r="H39" s="101" t="s">
+        <v>58</v>
       </c>
       <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="144">
+      <c r="A40" s="145">
         <f>A38 -1</f>
         <v>4</v>
       </c>
-      <c r="B40" s="128"/>
+      <c r="B40" s="146"/>
       <c r="C40" s="95">
         <f>I38 + 1</f>
         <v>10</v>
@@ -3034,18 +3008,18 @@
         <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="H40" s="110">
+      <c r="H40" s="108">
         <f t="shared" si="9"/>
         <v>15</v>
       </c>
-      <c r="I40" s="111">
+      <c r="I40" s="109">
         <f t="shared" si="9"/>
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="44.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="136"/>
-      <c r="B41" s="128"/>
+      <c r="A41" s="135"/>
+      <c r="B41" s="146"/>
       <c r="C41" s="38"/>
       <c r="D41" s="36" t="s">
         <v>7</v>
@@ -3055,24 +3029,24 @@
         <v>7</v>
       </c>
       <c r="G41" s="36"/>
-      <c r="H41" s="110" t="s">
+      <c r="H41" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="111" t="s">
+      <c r="I41" s="109" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="136">
+      <c r="A42" s="135">
         <f>A40 -1</f>
         <v>3</v>
       </c>
-      <c r="B42" s="128"/>
-      <c r="C42" s="110">
+      <c r="B42" s="146"/>
+      <c r="C42" s="108">
         <f>I40 + 1</f>
         <v>17</v>
       </c>
-      <c r="D42" s="110">
+      <c r="D42" s="108">
         <f>C42 + 1</f>
         <v>18</v>
       </c>
@@ -3098,30 +3072,30 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="136"/>
-      <c r="B43" s="128"/>
-      <c r="C43" s="115" t="s">
+      <c r="A43" s="135"/>
+      <c r="B43" s="146"/>
+      <c r="C43" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="109" t="s">
+      <c r="D43" s="107" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="56" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G43" s="23"/>
       <c r="H43" s="23" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="136">
+      <c r="A44" s="135">
         <f>A42 -1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="128"/>
+      <c r="B44" s="146"/>
       <c r="C44" s="38">
         <f>I42 + 1</f>
         <v>24</v>
@@ -3152,10 +3126,12 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="137"/>
-      <c r="B45" s="128"/>
+      <c r="A45" s="142"/>
+      <c r="B45" s="146"/>
       <c r="C45" s="88"/>
-      <c r="D45" s="57"/>
+      <c r="D45" s="57" t="s">
+        <v>7</v>
+      </c>
       <c r="E45" s="55"/>
       <c r="F45" s="57" t="s">
         <v>7</v>
@@ -3167,11 +3143,11 @@
       <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="138">
+      <c r="A46" s="132">
         <f>A44 -1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="129" t="s">
+      <c r="B46" s="147" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="34">
@@ -3203,8 +3179,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="139"/>
-      <c r="B47" s="130"/>
+      <c r="A47" s="131"/>
+      <c r="B47" s="136"/>
       <c r="C47" s="35"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -3215,17 +3191,17 @@
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I47" s="39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="143" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="140" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="130"/>
+      <c r="B48" s="136"/>
       <c r="C48" s="21">
         <f>I46 + 1</f>
         <v>8</v>
@@ -3246,35 +3222,50 @@
         <f t="shared" si="14"/>
         <v>12</v>
       </c>
-      <c r="H48" s="122">
+      <c r="H48" s="120">
         <f t="shared" si="14"/>
         <v>13</v>
       </c>
-      <c r="I48" s="123">
+      <c r="I48" s="121">
         <f t="shared" si="14"/>
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A49" s="141"/>
-      <c r="B49" s="131"/>
+      <c r="A49" s="144"/>
+      <c r="B49" s="137"/>
       <c r="C49" s="97" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E49" s="98"/>
       <c r="F49" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G49" s="22"/>
-      <c r="H49" s="124"/>
-      <c r="I49" s="125"/>
+      <c r="H49" s="122"/>
+      <c r="I49" s="123"/>
     </row>
     <row r="50" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -3288,21 +3279,6 @@
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="98" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
swapped testing and SQL Labs review
</commit_message>
<xml_diff>
--- a/CS320-Spring2022Calendar.xlsx
+++ b/CS320-Spring2022Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D20F60-1FE0-4B0D-ADF7-2C84C002534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D20AFC-CEC0-4376-94DB-4CFE941B4301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1098" yWindow="978" windowWidth="21714" windowHeight="11982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9102" yWindow="270" windowWidth="13818" windowHeight="11982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp22" sheetId="1" r:id="rId1"/>
@@ -433,10 +433,6 @@
 due (7:00a)
 ** full credit **
 (Marmoset)</t>
-  </si>
-  <si>
-    <t>CS320: SW Engineering - Spring 2022 Schedule
-(as of 3-22-2022, subject to change)</t>
   </si>
   <si>
     <t xml:space="preserve">Library Example Project
@@ -550,6 +546,10 @@
     <t xml:space="preserve">Lab 6: ORM due  7:00 am
 *10% extra credit* (Marmoset)
 </t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2022 Schedule
+(as of 3-26-2022, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1631,35 +1631,23 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1667,6 +1655,60 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1677,48 +1719,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2064,8 +2064,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2083,17 +2083,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="125" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="127"/>
+      <c r="A1" s="146" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="148"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
@@ -2123,10 +2123,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="131">
+      <c r="A3" s="139">
         <v>15</v>
       </c>
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="107">
@@ -2158,8 +2158,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="130"/>
-      <c r="B4" s="147"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="133"/>
       <c r="C4" s="109" t="s">
         <v>8</v>
       </c>
@@ -2185,11 +2185,11 @@
       <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="130">
+      <c r="A5" s="140">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="131" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="8">
@@ -2221,8 +2221,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="132"/>
-      <c r="B6" s="136"/>
+      <c r="A6" s="143"/>
+      <c r="B6" s="132"/>
       <c r="C6" s="68"/>
       <c r="D6" s="62" t="s">
         <v>47</v>
@@ -2240,11 +2240,11 @@
       <c r="I6" s="69"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="133">
+      <c r="A7" s="144">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="151" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="51">
@@ -2277,8 +2277,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="134"/>
-      <c r="B8" s="138"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="152"/>
       <c r="C8" s="40" t="s">
         <v>58</v>
       </c>
@@ -2296,11 +2296,11 @@
       <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="134">
+      <c r="A9" s="137">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="138"/>
+      <c r="B9" s="152"/>
       <c r="C9" s="15">
         <f>I7 + 1</f>
         <v>13</v>
@@ -2331,8 +2331,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="90.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="134"/>
-      <c r="B10" s="138"/>
+      <c r="A10" s="137"/>
+      <c r="B10" s="152"/>
       <c r="C10" s="67" t="s">
         <v>35</v>
       </c>
@@ -2350,11 +2350,11 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="134">
+      <c r="A11" s="137">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="138"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="18">
         <f>I9 + 1</f>
         <v>20</v>
@@ -2385,8 +2385,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="90.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="134"/>
-      <c r="B12" s="138"/>
+      <c r="A12" s="137"/>
+      <c r="B12" s="152"/>
       <c r="C12" s="40" t="s">
         <v>44</v>
       </c>
@@ -2404,11 +2404,11 @@
       <c r="I12" s="120"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="139">
+      <c r="A13" s="153">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="134" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="18">
@@ -2440,8 +2440,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="107.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="140"/>
-      <c r="B14" s="149"/>
+      <c r="A14" s="154"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="38"/>
       <c r="D14" s="99" t="s">
         <v>30</v>
@@ -2457,11 +2457,11 @@
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="131">
+      <c r="A15" s="139">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="135" t="s">
+      <c r="B15" s="131" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="74">
@@ -2494,8 +2494,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="132"/>
-      <c r="B16" s="136"/>
+      <c r="A16" s="143"/>
+      <c r="B16" s="132"/>
       <c r="C16" s="77" t="s">
         <v>49</v>
       </c>
@@ -2651,19 +2651,19 @@
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="125" t="str">
+      <c r="A28" s="146" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2022 Schedule
-(as of 3-22-2022, subject to change)</v>
-      </c>
-      <c r="B28" s="126"/>
-      <c r="C28" s="126"/>
-      <c r="D28" s="126"/>
-      <c r="E28" s="126"/>
-      <c r="F28" s="126"/>
-      <c r="G28" s="126"/>
-      <c r="H28" s="126"/>
-      <c r="I28" s="127"/>
+(as of 3-26-2022, subject to change)</v>
+      </c>
+      <c r="B28" s="147"/>
+      <c r="C28" s="147"/>
+      <c r="D28" s="147"/>
+      <c r="E28" s="147"/>
+      <c r="F28" s="147"/>
+      <c r="G28" s="147"/>
+      <c r="H28" s="147"/>
+      <c r="I28" s="148"/>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="str">
@@ -2701,11 +2701,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="128">
+      <c r="A30" s="149">
         <f>A15</f>
         <v>9</v>
       </c>
-      <c r="B30" s="146" t="s">
+      <c r="B30" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="87">
@@ -2738,8 +2738,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="129"/>
-      <c r="B31" s="135"/>
+      <c r="A31" s="150"/>
+      <c r="B31" s="131"/>
       <c r="C31" s="87" t="str">
         <f>C16</f>
         <v xml:space="preserve"> </v>
@@ -2777,11 +2777,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="129">
+      <c r="A32" s="150">
         <f xml:space="preserve"> A30 - 1</f>
         <v>8</v>
       </c>
-      <c r="B32" s="135"/>
+      <c r="B32" s="131"/>
       <c r="C32" s="106">
         <f>I15 + 1</f>
         <v>13</v>
@@ -2812,8 +2812,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="130"/>
-      <c r="B33" s="135"/>
+      <c r="A33" s="140"/>
+      <c r="B33" s="131"/>
       <c r="C33" s="40" t="s">
         <v>53</v>
       </c>
@@ -2831,11 +2831,11 @@
       <c r="I33" s="47"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="130">
+      <c r="A34" s="140">
         <f>A32 - 1</f>
         <v>7</v>
       </c>
-      <c r="B34" s="135"/>
+      <c r="B34" s="131"/>
       <c r="C34" s="21">
         <f>I32 + 1</f>
         <v>20</v>
@@ -2866,15 +2866,15 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="117.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="130"/>
-      <c r="B35" s="135"/>
+      <c r="A35" s="140"/>
+      <c r="B35" s="131"/>
       <c r="C35" s="66"/>
       <c r="D35" s="33" t="s">
         <v>32</v>
       </c>
       <c r="E35" s="80"/>
       <c r="F35" s="60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G35" s="124" t="s">
         <v>67</v>
@@ -2883,15 +2883,15 @@
         <v>66</v>
       </c>
       <c r="I35" s="123" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="130">
+      <c r="A36" s="140">
         <f>A34 - 1</f>
         <v>6</v>
       </c>
-      <c r="B36" s="150" t="s">
+      <c r="B36" s="136" t="s">
         <v>52</v>
       </c>
       <c r="C36" s="8">
@@ -2923,10 +2923,10 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="132"/>
-      <c r="B37" s="136"/>
+      <c r="A37" s="143"/>
+      <c r="B37" s="132"/>
       <c r="C37" s="95" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>27</v>
@@ -2935,22 +2935,22 @@
         <v>36</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="G37" s="93"/>
       <c r="H37" s="122" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="133">
+      <c r="A38" s="144">
         <f>A36 -1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="145" t="s">
+      <c r="B38" s="129" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="91">
@@ -2983,30 +2983,30 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="134"/>
-      <c r="B39" s="145"/>
-      <c r="C39" s="154" t="s">
-        <v>75</v>
+      <c r="A39" s="137"/>
+      <c r="B39" s="129"/>
+      <c r="C39" s="128" t="s">
+        <v>74</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E39" s="36"/>
       <c r="F39" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G39" s="153"/>
-      <c r="H39" s="152" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="G39" s="127"/>
+      <c r="H39" s="126" t="s">
+        <v>71</v>
       </c>
       <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="144">
+      <c r="A40" s="145">
         <f>A38 -1</f>
         <v>4</v>
       </c>
-      <c r="B40" s="145"/>
+      <c r="B40" s="129"/>
       <c r="C40" s="94">
         <f>I38 + 1</f>
         <v>10</v>
@@ -3037,8 +3037,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="44.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="134"/>
-      <c r="B41" s="145"/>
+      <c r="A41" s="137"/>
+      <c r="B41" s="129"/>
       <c r="C41" s="38"/>
       <c r="D41" s="36" t="s">
         <v>7</v>
@@ -3056,11 +3056,11 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="134">
+      <c r="A42" s="137">
         <f>A40 -1</f>
         <v>3</v>
       </c>
-      <c r="B42" s="145"/>
+      <c r="B42" s="129"/>
       <c r="C42" s="104">
         <f>I40 + 1</f>
         <v>17</v>
@@ -3091,8 +3091,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="134"/>
-      <c r="B43" s="145"/>
+      <c r="A43" s="137"/>
+      <c r="B43" s="129"/>
       <c r="C43" s="109" t="s">
         <v>6</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>6</v>
       </c>
       <c r="E43" s="12"/>
-      <c r="F43" s="151" t="s">
+      <c r="F43" s="125" t="s">
         <v>33</v>
       </c>
       <c r="G43" s="67" t="s">
@@ -3112,11 +3112,11 @@
       <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="134">
+      <c r="A44" s="137">
         <f>A42 -1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="145"/>
+      <c r="B44" s="129"/>
       <c r="C44" s="38">
         <f>I42 + 1</f>
         <v>24</v>
@@ -3147,8 +3147,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="141"/>
-      <c r="B45" s="145"/>
+      <c r="A45" s="138"/>
+      <c r="B45" s="129"/>
       <c r="C45" s="88"/>
       <c r="D45" s="56" t="s">
         <v>29</v>
@@ -3164,11 +3164,11 @@
       <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="131">
+      <c r="A46" s="139">
         <f>A44 -1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="146" t="s">
+      <c r="B46" s="130" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="34">
@@ -3200,8 +3200,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="130"/>
-      <c r="B47" s="135"/>
+      <c r="A47" s="140"/>
+      <c r="B47" s="131"/>
       <c r="C47" s="35"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -3219,10 +3219,10 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="142" t="s">
+      <c r="A48" s="141" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="135"/>
+      <c r="B48" s="131"/>
       <c r="C48" s="21">
         <f>I46 + 1</f>
         <v>8</v>
@@ -3253,8 +3253,8 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A49" s="143"/>
-      <c r="B49" s="136"/>
+      <c r="A49" s="142"/>
+      <c r="B49" s="132"/>
       <c r="C49" s="95" t="s">
         <v>39</v>
       </c>
@@ -3272,21 +3272,6 @@
     <row r="50" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -3300,6 +3285,21 @@
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="98" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates to schedule for Lecture 17 and Individual Project Report
</commit_message>
<xml_diff>
--- a/CS320-Spring2022Calendar.xlsx
+++ b/CS320-Spring2022Calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D20AFC-CEC0-4376-94DB-4CFE941B4301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E7440C-6F9E-4DDA-BF8D-EA1FC4DAEE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9102" yWindow="270" windowWidth="13818" windowHeight="11982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="420" windowWidth="22620" windowHeight="11556" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp22" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="77">
   <si>
     <t>Monday</t>
   </si>
@@ -181,15 +181,6 @@
   <si>
     <t>A11: Team Project Midterm
 Peer Evals due
-7:00 am
-(Marmoset)</t>
-  </si>
-  <si>
-    <t>A09: Individual Code &amp; Report due 7:00 am
-(Marmoset)</t>
-  </si>
-  <si>
-    <t>A08: Team Code and Report due 
 7:00 am
 (Marmoset)</t>
   </si>
@@ -406,10 +397,6 @@
 (in-class)</t>
   </si>
   <si>
-    <t>Lecture 16: Testing
-Lecture 17: Quality Assurance</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Lecture  15: ORM, Designing a Persistence Layer
 </t>
@@ -433,32 +420,6 @@
 due (7:00a)
 ** full credit **
 (Marmoset)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Library Example Project
-Analysis and
-Review (part 1)
-</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Library Example Project
-Analysis and
-Review (part 2)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Take Home Exam
-(handed out)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -549,7 +510,56 @@
   </si>
   <si>
     <t>CS320: SW Engineering - Spring 2022 Schedule
-(as of 3-26-2022, subject to change)</t>
+(as of 4-14-2022, subject to change)</t>
+  </si>
+  <si>
+    <t>Lecture 16: Testing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Library Example Project
+Analysis and
+Review
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Take Home Exam
+(handed out)</t>
+    </r>
+  </si>
+  <si>
+    <t>Lecture 17: Quality Assurance</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Session
+(in class)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A09: Individual  Report due 7:00 am
+(Marmoset)</t>
+    </r>
+  </si>
+  <si>
+    <t>A08: Team Report due 7:00 am
+(Marmoset)</t>
   </si>
 </sst>
 </file>
@@ -1643,18 +1653,72 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1666,60 +1730,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2064,8 +2074,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2083,17 +2093,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="146" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="148"/>
+      <c r="A1" s="129" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="131"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
@@ -2123,10 +2133,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="139">
+      <c r="A3" s="135">
         <v>15</v>
       </c>
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="150" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="107">
@@ -2158,8 +2168,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="140"/>
-      <c r="B4" s="133"/>
+      <c r="A4" s="134"/>
+      <c r="B4" s="151"/>
       <c r="C4" s="109" t="s">
         <v>8</v>
       </c>
@@ -2185,12 +2195,12 @@
       <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="140">
+      <c r="A5" s="134">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="131" t="s">
-        <v>50</v>
+      <c r="B5" s="139" t="s">
+        <v>48</v>
       </c>
       <c r="C5" s="8">
         <f>I3 + 1</f>
@@ -2221,30 +2231,30 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="143"/>
-      <c r="B6" s="132"/>
+      <c r="A6" s="136"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="68"/>
       <c r="D6" s="62" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="86"/>
       <c r="F6" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G6" s="67" t="s">
         <v>34</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I6" s="69"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="144">
+      <c r="A7" s="137">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="151" t="s">
+      <c r="B7" s="141" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="51">
@@ -2277,30 +2287,30 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="137"/>
-      <c r="B8" s="152"/>
+      <c r="A8" s="138"/>
+      <c r="B8" s="142"/>
       <c r="C8" s="40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="137">
+      <c r="A9" s="138">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="152"/>
+      <c r="B9" s="142"/>
       <c r="C9" s="15">
         <f>I7 + 1</f>
         <v>13</v>
@@ -2331,8 +2341,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="90.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="137"/>
-      <c r="B10" s="152"/>
+      <c r="A10" s="138"/>
+      <c r="B10" s="142"/>
       <c r="C10" s="67" t="s">
         <v>35</v>
       </c>
@@ -2345,16 +2355,16 @@
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="137">
+      <c r="A11" s="138">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="152"/>
+      <c r="B11" s="142"/>
       <c r="C11" s="18">
         <f>I9 + 1</f>
         <v>20</v>
@@ -2385,17 +2395,17 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="90.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="137"/>
-      <c r="B12" s="152"/>
+      <c r="A12" s="138"/>
+      <c r="B12" s="142"/>
       <c r="C12" s="40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E12" s="63"/>
       <c r="F12" s="63" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G12" s="85"/>
       <c r="H12" s="121" t="s">
@@ -2404,12 +2414,12 @@
       <c r="I12" s="120"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="153">
+      <c r="A13" s="143">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="134" t="s">
-        <v>51</v>
+      <c r="B13" s="152" t="s">
+        <v>49</v>
       </c>
       <c r="C13" s="18">
         <f>I11 + 1</f>
@@ -2440,28 +2450,28 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="107.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="154"/>
-      <c r="B14" s="135"/>
+      <c r="A14" s="144"/>
+      <c r="B14" s="153"/>
       <c r="C14" s="38"/>
       <c r="D14" s="99" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="82"/>
       <c r="F14" s="64" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G14" s="78"/>
       <c r="H14" s="49" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="139">
+      <c r="A15" s="135">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="139" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="74">
@@ -2494,22 +2504,22 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="143"/>
-      <c r="B16" s="132"/>
+      <c r="A16" s="136"/>
+      <c r="B16" s="140"/>
       <c r="C16" s="77" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="98" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G16" s="112" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H16" s="113" t="str">
         <f>G16</f>
@@ -2599,7 +2609,7 @@
       <c r="C23" s="41"/>
       <c r="D23" s="30"/>
       <c r="E23" s="97" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
@@ -2651,19 +2661,19 @@
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="146" t="str">
+      <c r="A28" s="129" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2022 Schedule
-(as of 3-26-2022, subject to change)</v>
-      </c>
-      <c r="B28" s="147"/>
-      <c r="C28" s="147"/>
-      <c r="D28" s="147"/>
-      <c r="E28" s="147"/>
-      <c r="F28" s="147"/>
-      <c r="G28" s="147"/>
-      <c r="H28" s="147"/>
-      <c r="I28" s="148"/>
+(as of 4-14-2022, subject to change)</v>
+      </c>
+      <c r="B28" s="130"/>
+      <c r="C28" s="130"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="131"/>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="str">
@@ -2701,11 +2711,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="149">
+      <c r="A30" s="132">
         <f>A15</f>
         <v>9</v>
       </c>
-      <c r="B30" s="130" t="s">
+      <c r="B30" s="150" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="87">
@@ -2738,8 +2748,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="150"/>
-      <c r="B31" s="131"/>
+      <c r="A31" s="133"/>
+      <c r="B31" s="139"/>
       <c r="C31" s="87" t="str">
         <f>C16</f>
         <v xml:space="preserve"> </v>
@@ -2777,11 +2787,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="150">
+      <c r="A32" s="133">
         <f xml:space="preserve"> A30 - 1</f>
         <v>8</v>
       </c>
-      <c r="B32" s="131"/>
+      <c r="B32" s="139"/>
       <c r="C32" s="106">
         <f>I15 + 1</f>
         <v>13</v>
@@ -2812,10 +2822,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="140"/>
-      <c r="B33" s="131"/>
+      <c r="A33" s="134"/>
+      <c r="B33" s="139"/>
       <c r="C33" s="40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>15</v>
@@ -2831,11 +2841,11 @@
       <c r="I33" s="47"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="140">
+      <c r="A34" s="134">
         <f>A32 - 1</f>
         <v>7</v>
       </c>
-      <c r="B34" s="131"/>
+      <c r="B34" s="139"/>
       <c r="C34" s="21">
         <f>I32 + 1</f>
         <v>20</v>
@@ -2866,33 +2876,33 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="117.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="140"/>
-      <c r="B35" s="131"/>
+      <c r="A35" s="134"/>
+      <c r="B35" s="139"/>
       <c r="C35" s="66"/>
       <c r="D35" s="33" t="s">
         <v>32</v>
       </c>
       <c r="E35" s="80"/>
       <c r="F35" s="60" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G35" s="124" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="H35" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I35" s="123" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="140">
+      <c r="A36" s="134">
         <f>A34 - 1</f>
         <v>6</v>
       </c>
-      <c r="B36" s="136" t="s">
-        <v>52</v>
+      <c r="B36" s="154" t="s">
+        <v>50</v>
       </c>
       <c r="C36" s="8">
         <f>I34 + 1</f>
@@ -2923,10 +2933,10 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="143"/>
-      <c r="B37" s="132"/>
+      <c r="A37" s="136"/>
+      <c r="B37" s="140"/>
       <c r="C37" s="95" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>27</v>
@@ -2939,18 +2949,18 @@
       </c>
       <c r="G37" s="93"/>
       <c r="H37" s="122" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="144">
+      <c r="A38" s="137">
         <f>A36 -1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="129" t="s">
+      <c r="B38" s="149" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="91">
@@ -2983,30 +2993,30 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="137"/>
-      <c r="B39" s="129"/>
+      <c r="A39" s="138"/>
+      <c r="B39" s="149"/>
       <c r="C39" s="128" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="23" t="s">
         <v>74</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>68</v>
       </c>
       <c r="E39" s="36"/>
       <c r="F39" s="23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G39" s="127"/>
       <c r="H39" s="126" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="145">
+      <c r="A40" s="148">
         <f>A38 -1</f>
         <v>4</v>
       </c>
-      <c r="B40" s="129"/>
+      <c r="B40" s="149"/>
       <c r="C40" s="94">
         <f>I38 + 1</f>
         <v>10</v>
@@ -3037,8 +3047,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="44.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="137"/>
-      <c r="B41" s="129"/>
+      <c r="A41" s="138"/>
+      <c r="B41" s="149"/>
       <c r="C41" s="38"/>
       <c r="D41" s="36" t="s">
         <v>7</v>
@@ -3056,11 +3066,11 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="137">
+      <c r="A42" s="138">
         <f>A40 -1</f>
         <v>3</v>
       </c>
-      <c r="B42" s="129"/>
+      <c r="B42" s="149"/>
       <c r="C42" s="104">
         <f>I40 + 1</f>
         <v>17</v>
@@ -3090,9 +3100,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="137"/>
-      <c r="B43" s="129"/>
+    <row r="43" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="138"/>
+      <c r="B43" s="149"/>
       <c r="C43" s="109" t="s">
         <v>6</v>
       </c>
@@ -3103,20 +3113,18 @@
       <c r="F43" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="G43" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="H43" s="23" t="s">
-        <v>7</v>
+      <c r="G43" s="127"/>
+      <c r="H43" s="60" t="s">
+        <v>75</v>
       </c>
       <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="137">
+      <c r="A44" s="138">
         <f>A42 -1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="129"/>
+      <c r="B44" s="149"/>
       <c r="C44" s="38">
         <f>I42 + 1</f>
         <v>24</v>
@@ -3147,8 +3155,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="138"/>
-      <c r="B45" s="129"/>
+      <c r="A45" s="145"/>
+      <c r="B45" s="149"/>
       <c r="C45" s="88"/>
       <c r="D45" s="56" t="s">
         <v>29</v>
@@ -3164,11 +3172,11 @@
       <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="139">
+      <c r="A46" s="135">
         <f>A44 -1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="130" t="s">
+      <c r="B46" s="150" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="34">
@@ -3200,8 +3208,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="140"/>
-      <c r="B47" s="131"/>
+      <c r="A47" s="134"/>
+      <c r="B47" s="139"/>
       <c r="C47" s="35"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -3212,17 +3220,17 @@
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I47" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="146" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="141" t="s">
-        <v>40</v>
-      </c>
-      <c r="B48" s="131"/>
+      <c r="B48" s="139"/>
       <c r="C48" s="21">
         <f>I46 + 1</f>
         <v>8</v>
@@ -3253,17 +3261,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A49" s="142"/>
-      <c r="B49" s="132"/>
+      <c r="A49" s="147"/>
+      <c r="B49" s="140"/>
       <c r="C49" s="95" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E49" s="96"/>
       <c r="F49" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="118"/>
@@ -3272,6 +3280,21 @@
     <row r="50" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -3285,23 +3308,8 @@
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
-  <pageSetup paperSize="5" scale="98" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="96" fitToHeight="2" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>